<commit_message>
more local exp figures added
</commit_message>
<xml_diff>
--- a/data/data_test_1.xlsx
+++ b/data/data_test_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SImAge_Gradio\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5BDCEDD-BCEE-455A-98E8-E3113F020243}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45003C1D-C2CE-49C6-9935-9BA794B323B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2670" yWindow="4515" windowWidth="25125" windowHeight="16365" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2355" yWindow="1950" windowWidth="25125" windowHeight="16365" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -565,7 +565,7 @@
   <dimension ref="A1:BB2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>